<commit_message>
create basic solution test cases
</commit_message>
<xml_diff>
--- a/extras/skills_mapping.xlsx
+++ b/extras/skills_mapping.xlsx
@@ -1,37 +1,163 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcheam/Desktop/Projects/myProjects/automatic-roster/extras/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1525CDB-5E9D-544A-A8EB-09C5572FF04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>SOUND #1 (M)</t>
+  </si>
+  <si>
+    <t>PROJECTIONIST (M)</t>
+  </si>
+  <si>
+    <t>COORDINATOR (B)</t>
+  </si>
+  <si>
+    <t>LIVESTREAM #1 (B)</t>
+  </si>
+  <si>
+    <t>SOUND #1 (B)</t>
+  </si>
+  <si>
+    <t>SOUND #2 (B)</t>
+  </si>
+  <si>
+    <t>PROJECTIONIST (B)</t>
+  </si>
+  <si>
+    <t>ANDREW</t>
+  </si>
+  <si>
+    <t>CHEE FS</t>
+  </si>
+  <si>
+    <t>ELLY</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>FRED KWAN</t>
+  </si>
+  <si>
+    <t>HING GEE</t>
+  </si>
+  <si>
+    <t>HONGTO</t>
+  </si>
+  <si>
+    <t>IAN MING</t>
+  </si>
+  <si>
+    <t>JAIRUS</t>
+  </si>
+  <si>
+    <t>JEFFERY</t>
+  </si>
+  <si>
+    <t>JEREMY</t>
+  </si>
+  <si>
+    <t>JURINA</t>
+  </si>
+  <si>
+    <t>LAWRENCE</t>
+  </si>
+  <si>
+    <t>MATHIAS</t>
+  </si>
+  <si>
+    <t>MU TIAN</t>
+  </si>
+  <si>
+    <t>PAMELA CHEONG</t>
+  </si>
+  <si>
+    <t>SHAWN</t>
+  </si>
+  <si>
+    <t>SHERMAN</t>
+  </si>
+  <si>
+    <t>SIAW ENG</t>
+  </si>
+  <si>
+    <t>SINGYE</t>
+  </si>
+  <si>
+    <t>STEVEN</t>
+  </si>
+  <si>
+    <t>SWEE GEOK</t>
+  </si>
+  <si>
+    <t>TIMOTHY</t>
+  </si>
+  <si>
+    <t>TITUS</t>
+  </si>
+  <si>
+    <t>WEI XUAN</t>
+  </si>
+  <si>
+    <t>WONSEN</t>
+  </si>
+  <si>
+    <t>YU TANG</t>
+  </si>
+  <si>
+    <t>YU XUAN</t>
+  </si>
+  <si>
+    <t>ZHI QIAN</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +172,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,69 +496,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Names</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>SOUND #1 (M)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PROJECTIONIST (M)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>COORDINATOR (B)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>LIVESTREAM #1 (B)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>SOUND #1 (B)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>SOUND #2 (B)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>PROJECTIONIST (B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ANDREW</t>
-        </is>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -506,14 +569,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CHEE FS</t>
-        </is>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -537,14 +598,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ELLY</t>
-        </is>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -568,14 +627,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>FAM</t>
-        </is>
+      <c r="B5" t="s">
+        <v>11</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -599,14 +656,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>FRED KWAN</t>
-        </is>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -630,14 +685,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>HING GEE</t>
-        </is>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -661,14 +714,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>HONGTO</t>
-        </is>
+      <c r="B8" t="s">
+        <v>14</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -692,14 +743,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>IAN MING</t>
-        </is>
+      <c r="B9" t="s">
+        <v>15</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -723,14 +772,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JAIRUS</t>
-        </is>
+      <c r="B10" t="s">
+        <v>16</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -754,14 +801,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>JEFFERY</t>
-        </is>
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -785,14 +830,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>JEREMY</t>
-        </is>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -816,14 +859,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>JURINA</t>
-        </is>
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -847,14 +888,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>LAWRENCE</t>
-        </is>
+      <c r="B14" t="s">
+        <v>20</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -878,14 +917,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MATHIAS</t>
-        </is>
+      <c r="B15" t="s">
+        <v>21</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -909,14 +946,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>MU TIAN</t>
-        </is>
+      <c r="B16" t="s">
+        <v>22</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -940,14 +975,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>PAMELA CHEONG</t>
-        </is>
+      <c r="B17" t="s">
+        <v>23</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -971,14 +1004,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SHAWN</t>
-        </is>
+      <c r="B18" t="s">
+        <v>24</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1002,14 +1033,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>SHERMAN</t>
-        </is>
+      <c r="B19" t="s">
+        <v>25</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1033,14 +1062,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SIAW ENG</t>
-        </is>
+      <c r="B20" t="s">
+        <v>26</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1064,14 +1091,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SINGYE</t>
-        </is>
+      <c r="B21" t="s">
+        <v>27</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1095,14 +1120,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>STEVEN</t>
-        </is>
+      <c r="B22" t="s">
+        <v>28</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -1126,14 +1149,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>SWEE GEOK</t>
-        </is>
+      <c r="B23" t="s">
+        <v>29</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1157,14 +1178,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>TIMOTHY</t>
-        </is>
+      <c r="B24" t="s">
+        <v>30</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1188,14 +1207,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>TITUS</t>
-        </is>
+      <c r="B25" t="s">
+        <v>31</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -1219,14 +1236,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>WEI XUAN</t>
-        </is>
+      <c r="B26" t="s">
+        <v>32</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1250,14 +1265,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>WONSEN</t>
-        </is>
+      <c r="B27" t="s">
+        <v>33</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1281,14 +1294,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>YU TANG</t>
-        </is>
+      <c r="B28" t="s">
+        <v>34</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1312,14 +1323,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>YU XUAN</t>
-        </is>
+      <c r="B29" t="s">
+        <v>35</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1343,14 +1352,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>ZHI QIAN</t>
-        </is>
+      <c r="B30" t="s">
+        <v>36</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -1375,6 +1382,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>